<commit_message>
skenario paid course + fix testcase paid course
</commit_message>
<xml_diff>
--- a/configuration/AddCourseData.xlsx
+++ b/configuration/AddCourseData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ryu\github\SoftwareTesting\configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WILLIAM\OneDrive\Documents\s1Informatika\Semester_5\Softes\project\SoftwareTesting\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17BCEAF-4634-44E3-90A2-29C9D4134604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04075468-8423-4AA0-A15D-69EEE121A6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{833ED044-B85E-4044-8997-B73DDCA748A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{833ED044-B85E-4044-8997-B73DDCA748A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>Free</t>
+  </si>
+  <si>
+    <t>Paid</t>
   </si>
 </sst>
 </file>
@@ -592,43 +595,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5980D7E7-253F-433D-B6D4-DDB5750F4934}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="1"/>
-    <col min="2" max="2" width="10.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.06640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.06640625" style="1"/>
-    <col min="20" max="20" width="7.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="32.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.109375" style="1"/>
+    <col min="20" max="20" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.06640625" style="1"/>
+    <col min="28" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -794,7 +797,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -844,7 +847,7 @@
         <v>16</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>52</v>
@@ -877,7 +880,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
feat: report hasil instructor
</commit_message>
<xml_diff>
--- a/configuration/AddCourseData.xlsx
+++ b/configuration/AddCourseData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ryu\github\SoftwareTesting\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17BCEAF-4634-44E3-90A2-29C9D4134604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C525D077-8AEE-4D4C-95CC-0C3F46BF251B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{833ED044-B85E-4044-8997-B73DDCA748A6}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="16200" windowHeight="9308" xr2:uid="{833ED044-B85E-4044-8997-B73DDCA748A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>Free</t>
+  </si>
+  <si>
+    <t>Paid</t>
   </si>
 </sst>
 </file>
@@ -592,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5980D7E7-253F-433D-B6D4-DDB5750F4934}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -844,7 +847,7 @@
         <v>16</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>52</v>

</xml_diff>